<commit_message>
Nehogy tönkremenjen a gépem
</commit_message>
<xml_diff>
--- a/Termékek/Eszpresszó/Kulcsszavak/eRank - Eszpresszó.xlsx
+++ b/Termékek/Eszpresszó/Kulcsszavak/eRank - Eszpresszó.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkupi\Documents\Etsy ceramic\Termékek\Eszpresszó\Kulcsszavak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D81E076-52D4-411E-A85C-6F83E1905E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DACA89-7B5A-4C9B-9DA0-0822F12E7A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,12 +165,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -186,17 +192,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -216,9 +227,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 téma">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,7 +267,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -362,7 +373,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -504,7 +515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -512,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,20 +542,20 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -555,25 +566,25 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -584,26 +595,30 @@
         <v>128</v>
       </c>
       <c r="D3" s="4">
+        <v>728</v>
+      </c>
+      <c r="E3" s="8">
+        <f>C3/D3</f>
+        <v>0.17582417582417584</v>
+      </c>
+      <c r="F3" s="4">
         <v>189</v>
       </c>
-      <c r="E3" s="2">
+      <c r="G3" s="2">
         <v>1.48</v>
       </c>
-      <c r="F3" s="4">
-        <v>728</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>320</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="7">
-        <f>C3/F3</f>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="5">
+        <f>C3/D3</f>
         <v>0.17582417582417584</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -613,27 +628,31 @@
       <c r="C4" s="4">
         <v>391</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3">
+        <v>4258</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" ref="E4:E25" si="0">C4/D4</f>
+        <v>9.1827148896195393E-2</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3">
-        <v>4258</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>8100</v>
       </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="7">
-        <f t="shared" ref="I4:I25" si="0">C4/F4</f>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="5">
+        <f>C4/D4</f>
         <v>9.1827148896195393E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -643,57 +662,65 @@
       <c r="C5" s="4">
         <v>297</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
+        <v>3886</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>7.6428203808543496E-2</v>
+      </c>
+      <c r="F5" s="4">
         <v>434</v>
       </c>
-      <c r="E5" s="2">
+      <c r="G5" s="2">
         <v>1.46</v>
       </c>
-      <c r="F5" s="3">
-        <v>3886</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>2400</v>
       </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="7">
-        <f t="shared" si="0"/>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="5">
+        <f>C5/D5</f>
         <v>7.6428203808543496E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="10">
         <v>20</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="10">
         <v>147</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="11">
+        <v>7075</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0777385159010602E-2</v>
+      </c>
+      <c r="F6" s="10">
         <v>138</v>
       </c>
-      <c r="E6" s="2">
+      <c r="G6" s="12">
         <v>0.94</v>
       </c>
-      <c r="F6" s="3">
-        <v>7075</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="H6" s="11">
         <v>1600</v>
       </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="7">
-        <f t="shared" si="0"/>
+      <c r="I6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="8">
+        <f>C6/D6</f>
         <v>2.0777385159010602E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -704,56 +731,64 @@
         <v>10146</v>
       </c>
       <c r="D7" s="3">
+        <v>1464442</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>6.9282361472834024E-3</v>
+      </c>
+      <c r="F7" s="3">
         <v>10110</v>
       </c>
-      <c r="E7" s="2">
+      <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="F7" s="3">
-        <v>1464442</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>8100</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="7">
-        <f t="shared" si="0"/>
+      <c r="J7" s="5">
+        <f>C7/D7</f>
         <v>6.9282361472834024E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="10">
         <v>20</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="10">
         <v>557</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="11">
+        <v>2522</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.22085646312450435</v>
+      </c>
+      <c r="F8" s="10">
         <v>603</v>
       </c>
-      <c r="E8" s="2">
+      <c r="G8" s="12">
         <v>1.08</v>
       </c>
-      <c r="F8" s="3">
-        <v>2522</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="H8" s="11">
         <v>3600</v>
       </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="7">
-        <f t="shared" si="0"/>
+      <c r="I8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="8">
+        <f>C8/D8</f>
         <v>0.22085646312450435</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -764,26 +799,30 @@
         <v>3723</v>
       </c>
       <c r="D9" s="3">
+        <v>14754</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.25233834892232615</v>
+      </c>
+      <c r="F9" s="3">
         <v>4642</v>
       </c>
-      <c r="E9" s="2">
+      <c r="G9" s="2">
         <v>1.25</v>
       </c>
-      <c r="F9" s="3">
-        <v>14754</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>27100</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="7">
-        <f t="shared" si="0"/>
+      <c r="J9" s="5">
+        <f>C9/D9</f>
         <v>0.25233834892232615</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -793,27 +832,31 @@
       <c r="C10">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3">
+        <v>3633</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>5.5050922102945227E-3</v>
+      </c>
+      <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="3">
-        <v>3633</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>1900</v>
       </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="7">
-        <f t="shared" si="0"/>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="5">
+        <f>C10/D10</f>
         <v>5.5050922102945227E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -823,27 +866,31 @@
       <c r="C11" s="4">
         <v>265</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
+        <v>5441</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>4.8704282301047598E-2</v>
+      </c>
+      <c r="F11" s="4">
         <v>305</v>
       </c>
-      <c r="E11" s="2">
+      <c r="G11" s="2">
         <v>1.1499999999999999</v>
       </c>
-      <c r="F11" s="3">
-        <v>5441</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>4400</v>
       </c>
-      <c r="H11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="7">
-        <f t="shared" si="0"/>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="5">
+        <f>C11/D11</f>
         <v>4.8704282301047598E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -854,26 +901,30 @@
         <v>57</v>
       </c>
       <c r="D12" s="4">
+        <v>969</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="F12" s="4">
         <v>52</v>
       </c>
-      <c r="E12" s="2">
+      <c r="G12" s="2">
         <v>0.91</v>
       </c>
-      <c r="F12" s="4">
-        <v>969</v>
-      </c>
-      <c r="G12" s="4">
+      <c r="H12" s="4">
         <v>70</v>
       </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="7">
-        <f t="shared" si="0"/>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="5">
+        <f>C12/D12</f>
         <v>5.8823529411764705E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -883,27 +934,31 @@
       <c r="C13" s="4">
         <v>628</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
+        <v>14905</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>4.2133512244213349E-2</v>
+      </c>
+      <c r="F13" s="4">
         <v>830</v>
       </c>
-      <c r="E13" s="2">
+      <c r="G13" s="2">
         <v>1.32</v>
       </c>
-      <c r="F13" s="3">
-        <v>14905</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>27100</v>
       </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="7">
-        <f t="shared" si="0"/>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="5">
+        <f>C13/D13</f>
         <v>4.2133512244213349E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -913,27 +968,31 @@
       <c r="C14" s="4">
         <v>92</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
+        <v>1482</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>6.2078272604588397E-2</v>
+      </c>
+      <c r="F14" s="4">
         <v>92</v>
       </c>
-      <c r="E14" s="2">
+      <c r="G14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="3">
-        <v>1482</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>27100</v>
       </c>
-      <c r="H14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="7">
-        <f t="shared" si="0"/>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="5">
+        <f>C14/D14</f>
         <v>6.2078272604588397E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -944,26 +1003,30 @@
         <v>1092</v>
       </c>
       <c r="D15" s="3">
+        <v>50811</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1491409340497137E-2</v>
+      </c>
+      <c r="F15" s="3">
         <v>1438</v>
       </c>
-      <c r="E15" s="2">
+      <c r="G15" s="2">
         <v>1.32</v>
       </c>
-      <c r="F15" s="3">
-        <v>50811</v>
-      </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>2400</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="7">
-        <f t="shared" si="0"/>
+      <c r="J15" s="5">
+        <f>C15/D15</f>
         <v>2.1491409340497137E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -973,27 +1036,31 @@
       <c r="C16" s="4">
         <v>122</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
+        <v>1943</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" si="0"/>
+        <v>6.2789500772002058E-2</v>
+      </c>
+      <c r="F16" s="4">
         <v>175</v>
       </c>
-      <c r="E16" s="2">
+      <c r="G16" s="2">
         <v>1.43</v>
       </c>
-      <c r="F16" s="3">
-        <v>1943</v>
-      </c>
-      <c r="G16" s="4">
+      <c r="H16" s="4">
         <v>320</v>
       </c>
-      <c r="H16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="7">
-        <f t="shared" si="0"/>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="5">
+        <f>C16/D16</f>
         <v>6.2789500772002058E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1004,26 +1071,30 @@
         <v>1420</v>
       </c>
       <c r="D17" s="3">
+        <v>77914</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" si="0"/>
+        <v>1.8225222681417973E-2</v>
+      </c>
+      <c r="F17" s="3">
         <v>1609</v>
       </c>
-      <c r="E17" s="2">
+      <c r="G17" s="2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="F17" s="3">
-        <v>77914</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>2400</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="7">
-        <f t="shared" si="0"/>
+      <c r="J17" s="5">
+        <f>C17/D17</f>
         <v>1.8225222681417973E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1034,26 +1105,30 @@
         <v>22552</v>
       </c>
       <c r="D18" s="3">
+        <v>1178353</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" si="0"/>
+        <v>1.9138577319360157E-2</v>
+      </c>
+      <c r="F18" s="3">
         <v>22119</v>
       </c>
-      <c r="E18" s="2">
+      <c r="G18" s="2">
         <v>0.98</v>
       </c>
-      <c r="F18" s="3">
-        <v>1178353</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>74000</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="7">
-        <f t="shared" si="0"/>
+      <c r="J18" s="5">
+        <f>C18/D18</f>
         <v>1.9138577319360157E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1064,26 +1139,30 @@
         <v>2765</v>
       </c>
       <c r="D19" s="3">
+        <v>49214</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" si="0"/>
+        <v>5.6183199902466778E-2</v>
+      </c>
+      <c r="F19" s="3">
         <v>2862</v>
       </c>
-      <c r="E19" s="2">
+      <c r="G19" s="2">
         <v>1.04</v>
       </c>
-      <c r="F19" s="3">
-        <v>49214</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="H19" s="3">
         <v>2900</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="7">
-        <f t="shared" si="0"/>
+      <c r="J19" s="5">
+        <f>C19/D19</f>
         <v>5.6183199902466778E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1093,27 +1172,31 @@
       <c r="C20" s="4">
         <v>92</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
+        <v>8999</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0223358150905656E-2</v>
+      </c>
+      <c r="F20" s="4">
         <v>92</v>
       </c>
-      <c r="E20" s="2">
+      <c r="G20" s="2">
         <v>1</v>
       </c>
-      <c r="F20" s="3">
-        <v>8999</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3">
         <v>1600</v>
       </c>
-      <c r="H20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="7">
-        <f t="shared" si="0"/>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="5">
+        <f>C20/D20</f>
         <v>1.0223358150905656E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1124,26 +1207,30 @@
         <v>1253</v>
       </c>
       <c r="D21" s="3">
+        <v>23032</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" si="0"/>
+        <v>5.4402570336922543E-2</v>
+      </c>
+      <c r="F21" s="3">
         <v>1154</v>
       </c>
-      <c r="E21" s="2">
+      <c r="G21" s="2">
         <v>0.92</v>
       </c>
-      <c r="F21" s="3">
-        <v>23032</v>
-      </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>2900</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="7">
-        <f t="shared" si="0"/>
+      <c r="J21" s="5">
+        <f>C21/D21</f>
         <v>5.4402570336922543E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1153,27 +1240,31 @@
       <c r="C22" s="4">
         <v>105</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
+        <v>3141</v>
+      </c>
+      <c r="E22" s="8">
+        <f t="shared" si="0"/>
+        <v>3.3428844317096466E-2</v>
+      </c>
+      <c r="F22" s="4">
         <v>145</v>
       </c>
-      <c r="E22" s="2">
+      <c r="G22" s="2">
         <v>1.38</v>
       </c>
-      <c r="F22" s="3">
-        <v>3141</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="H22" s="3">
         <v>40500</v>
       </c>
-      <c r="H22" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="7">
-        <f t="shared" si="0"/>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="5">
+        <f>C22/D22</f>
         <v>3.3428844317096466E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1183,27 +1274,31 @@
       <c r="C23" s="4">
         <v>118</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
+        <v>1412</v>
+      </c>
+      <c r="E23" s="8">
+        <f t="shared" si="0"/>
+        <v>8.3569405099150146E-2</v>
+      </c>
+      <c r="F23" s="4">
         <v>171</v>
       </c>
-      <c r="E23" s="2">
+      <c r="G23" s="2">
         <v>1.45</v>
       </c>
-      <c r="F23" s="3">
-        <v>1412</v>
-      </c>
-      <c r="G23" s="4">
+      <c r="H23" s="4">
         <v>720</v>
       </c>
-      <c r="H23" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="7">
-        <f t="shared" si="0"/>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="5">
+        <f>C23/D23</f>
         <v>8.3569405099150146E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1214,26 +1309,30 @@
         <v>378</v>
       </c>
       <c r="D24" s="4">
+        <v>932</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" si="0"/>
+        <v>0.40557939914163088</v>
+      </c>
+      <c r="F24" s="4">
         <v>483</v>
       </c>
-      <c r="E24" s="2">
+      <c r="G24" s="2">
         <v>1.28</v>
       </c>
-      <c r="F24" s="4">
-        <v>932</v>
-      </c>
-      <c r="G24" s="3">
+      <c r="H24" s="3">
         <v>1600</v>
       </c>
-      <c r="H24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="7">
-        <f t="shared" si="0"/>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="5">
+        <f>C24/D24</f>
         <v>0.40557939914163088</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1244,22 +1343,26 @@
         <v>5390</v>
       </c>
       <c r="D25" s="3">
+        <v>1582865</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="0"/>
+        <v>3.4052177538829906E-3</v>
+      </c>
+      <c r="F25" s="3">
         <v>5692</v>
       </c>
-      <c r="E25" s="2">
+      <c r="G25" s="2">
         <v>1.06</v>
       </c>
-      <c r="F25" s="3">
-        <v>1582865</v>
-      </c>
-      <c r="G25" s="3">
+      <c r="H25" s="3">
         <v>6600</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>17</v>
       </c>
-      <c r="I25" s="7">
-        <f t="shared" si="0"/>
+      <c r="J25" s="5">
+        <f>C25/D25</f>
         <v>3.4052177538829906E-3</v>
       </c>
     </row>

</xml_diff>